<commit_message>
PCB rev 1.0 added. Minor modifications to the libraries and schematics
</commit_message>
<xml_diff>
--- a/STM32L031_TSSOP20_Dev_Board/Project Outputs for STM32L031_TSSOP20_Dev_Board/STM32L031_TSSOP20_Dev_Board_rev_1.0.xlsx
+++ b/STM32L031_TSSOP20_Dev_Board/Project Outputs for STM32L031_TSSOP20_Dev_Board/STM32L031_TSSOP20_Dev_Board_rev_1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\javi_\GitHub\STM32L031_TSSOP20_Dev_Board\STM32L031_TSSOP20_Dev_Board\Project Outputs for STM32L031_TSSOP20_Dev_Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEBA6631-82D4-48F6-A84F-37161E991AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0B3B75C-03D7-414B-BEBD-FD36A3177C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17580" yWindow="2175" windowWidth="17355" windowHeight="17865" xr2:uid="{713C2E8B-EE46-4232-8720-E6123A31DE71}"/>
+    <workbookView xWindow="17580" yWindow="2175" windowWidth="17355" windowHeight="17865" xr2:uid="{F8A98FFF-CB54-4D36-BA4E-59717F715F4D}"/>
   </bookViews>
   <sheets>
     <sheet name="STM32L031_TSSOP20_Dev_Board_rev" sheetId="1" r:id="rId1"/>
@@ -238,7 +238,7 @@
     <t>SB1</t>
   </si>
   <si>
-    <t>FC-135_32.7680KA-AG5</t>
+    <t>Q13FC1350000200</t>
   </si>
   <si>
     <t>Crystal</t>
@@ -623,7 +623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A21056-EE7D-4F58-8BF4-497B4939EED6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC00CE9E-7D24-452C-AEDD-0D7B4336BC0F}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
LDO replaced due to availability issues. Layout updated as well
</commit_message>
<xml_diff>
--- a/STM32L031_TSSOP20_Dev_Board/Project Outputs for STM32L031_TSSOP20_Dev_Board/STM32L031_TSSOP20_Dev_Board_rev_1.0.xlsx
+++ b/STM32L031_TSSOP20_Dev_Board/Project Outputs for STM32L031_TSSOP20_Dev_Board/STM32L031_TSSOP20_Dev_Board_rev_1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\javi_\GitHub\STM32L031_TSSOP20_Dev_Board\STM32L031_TSSOP20_Dev_Board\Project Outputs for STM32L031_TSSOP20_Dev_Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0B3B75C-03D7-414B-BEBD-FD36A3177C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{838BFFA1-D15C-49B9-B2E3-BFFE6243C916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17580" yWindow="2175" windowWidth="17355" windowHeight="17865" xr2:uid="{F8A98FFF-CB54-4D36-BA4E-59717F715F4D}"/>
+    <workbookView xWindow="17580" yWindow="2175" windowWidth="17355" windowHeight="17865" xr2:uid="{CA8358E1-CA36-42B8-92DA-EA018F847C60}"/>
   </bookViews>
   <sheets>
     <sheet name="STM32L031_TSSOP20_Dev_Board_rev" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
     <t>IC1</t>
   </si>
   <si>
-    <t>AP2120N-3.3TRG1</t>
+    <t>MIC5365-3.3YC5-TR</t>
   </si>
   <si>
     <t>LDO</t>
@@ -184,7 +184,7 @@
     <t>LED</t>
   </si>
   <si>
-    <t>LED1</t>
+    <t>LD1</t>
   </si>
   <si>
     <t>Yellow/20mA</t>
@@ -193,7 +193,7 @@
     <t>LTST-C171KGKT</t>
   </si>
   <si>
-    <t>LED2</t>
+    <t>LD2</t>
   </si>
   <si>
     <t>Green/20mA</t>
@@ -623,7 +623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC00CE9E-7D24-452C-AEDD-0D7B4336BC0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3675E312-8D34-45C8-ADE0-0752883F32B2}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
CN5 3D model fixed. 3V3 LDO replaced.
</commit_message>
<xml_diff>
--- a/STM32L031_TSSOP20_Dev_Board/Project Outputs for STM32L031_TSSOP20_Dev_Board/STM32L031_TSSOP20_Dev_Board_rev_1.0.xlsx
+++ b/STM32L031_TSSOP20_Dev_Board/Project Outputs for STM32L031_TSSOP20_Dev_Board/STM32L031_TSSOP20_Dev_Board_rev_1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\javi_\GitHub\STM32L031_TSSOP20_Dev_Board\STM32L031_TSSOP20_Dev_Board\Project Outputs for STM32L031_TSSOP20_Dev_Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javi_\GitHub\STM32L031_TSSOP20_Dev_Board\STM32L031_TSSOP20_Dev_Board\Project Outputs for STM32L031_TSSOP20_Dev_Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C34AD42-4B4C-44EC-AE74-EE7C806603D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A275F8E6-15B7-4363-867F-1F82407250EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17580" yWindow="2175" windowWidth="17355" windowHeight="17865" xr2:uid="{78709CE6-DED3-4BF5-A683-74965C5766BA}"/>
+    <workbookView xWindow="9255" yWindow="930" windowWidth="23550" windowHeight="16410" xr2:uid="{FBEC02B1-4680-4F4D-B5FB-0A944BE98383}"/>
   </bookViews>
   <sheets>
     <sheet name="STM32L031_TSSOP20_Dev_Board_rev" sheetId="1" r:id="rId1"/>
@@ -121,6 +121,12 @@
     <t>CN4</t>
   </si>
   <si>
+    <t>CN_5PIN</t>
+  </si>
+  <si>
+    <t>CN5</t>
+  </si>
+  <si>
     <t>RB715UMTL</t>
   </si>
   <si>
@@ -151,7 +157,7 @@
     <t>IC1</t>
   </si>
   <si>
-    <t>MIC5365-3.3YC5-TR</t>
+    <t>MIC5366-3.3YC5-TR</t>
   </si>
   <si>
     <t>LDO</t>
@@ -172,12 +178,6 @@
     <t>1.8V/150mA</t>
   </si>
   <si>
-    <t>CN_5PIN</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
     <t>LTST-C171KSKT</t>
   </si>
   <si>
@@ -220,7 +220,7 @@
     <t>510</t>
   </si>
   <si>
-    <t>SKRPABE010</t>
+    <t>PTS815_SJM_250_SMTR_LFS</t>
   </si>
   <si>
     <t>Switch</t>
@@ -623,7 +623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAB2893-F7F1-4EF6-BF70-DCDECA4CFEC5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5351A412-6DF1-41BA-AFDA-B14D3E589E26}">
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -795,10 +795,10 @@
         <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -810,99 +810,99 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">

</xml_diff>